<commit_message>
Fixed freeze traps and multiple people acting at once
</commit_message>
<xml_diff>
--- a/maze-gen/mazes/Maze.xlsx
+++ b/maze-gen/mazes/Maze.xlsx
@@ -5,15 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Copy of Sheet1" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Copy of Sheet1 1" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Copy of Sheet1 1_2" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Copy of Sheet1 1_2_2" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Copy of Sheet1 1_2_2_2" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -169,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -211,6 +213,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,7 +490,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1177,8 +1191,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P26" activeCellId="0" sqref="P26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1337,6 +1351,428 @@
       <c r="A14" s="1"/>
       <c r="F14" s="1"/>
       <c r="K14" s="3"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="3.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16374" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="J14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="3.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16374" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="K14" s="13"/>
       <c r="O14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>